<commit_message>
Versión previa a correcciones finales
</commit_message>
<xml_diff>
--- a/Documentos/Elementos.xlsx
+++ b/Documentos/Elementos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tesis\V1\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tesis\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9581CB10-BFF4-474E-9802-2574C7F15A33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671FE97D-4B53-45A8-B585-DC9BFA03AEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{235F467F-1802-4911-823F-393BAAD41149}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{235F467F-1802-4911-823F-393BAAD41149}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Fases Metodológicas</t>
   </si>
@@ -76,37 +76,112 @@
     <t>7. Validar el comportamiento del algoritmo en ambientes topológicos distintos.</t>
   </si>
   <si>
-    <t>Análisis de modelos SIS y SIR</t>
-  </si>
-  <si>
-    <t>Definición e implementación del sistema de vecindades</t>
-  </si>
-  <si>
-    <t>Diseño e implementación de reglas de comportamiento (individuos y enfermedad)</t>
-  </si>
-  <si>
-    <t>Definición de métricas</t>
-  </si>
-  <si>
-    <t>Diseño del algoritmo de clasificación en redes neuronales</t>
-  </si>
-  <si>
-    <t>Entrenamiento del algoritmo</t>
-  </si>
-  <si>
-    <t>Diseño e implementación de los escenarios de prueba</t>
-  </si>
-  <si>
-    <t>Aplicación de pruebas en el algoritmo en redes neuronales y conclusiones</t>
-  </si>
-  <si>
-    <t>Redacción del documento del trabajo de grado</t>
-  </si>
-  <si>
     <t>Actividades a realizar</t>
   </si>
   <si>
     <t>Semanas de ejecución de cada actividad</t>
+  </si>
+  <si>
+    <t>Fase 1: Modelos basados en autómatas celulares para la simulación de una enfermedad</t>
+  </si>
+  <si>
+    <t>Etapas</t>
+  </si>
+  <si>
+    <t>3. Implementación de reglas de comportamiento</t>
+  </si>
+  <si>
+    <t>4. Simulación del comportamiento de la enfermedad</t>
+  </si>
+  <si>
+    <t>2. Diseño de reglas probabilísticas para el comportamiento de la enfermedad en autómatas celulares</t>
+  </si>
+  <si>
+    <t>5. Obtención de datos para el algoritmo en redes neuronales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Análisis del impacto de la condición de frontera </t>
+  </si>
+  <si>
+    <t>8. Revisión de métodos de clasificación en redes neuronales</t>
+  </si>
+  <si>
+    <t>9. Definición de métricas para el algoritmo en redes neuronales</t>
+  </si>
+  <si>
+    <t>10. Diseño e implementación del algoritmo en redes neuronales sobre los datos simulados</t>
+  </si>
+  <si>
+    <t>11. Validación del comportamiento del algoritmo con los datos previamente simulados</t>
+  </si>
+  <si>
+    <t>13. Cambios de topología sobre la simulación en autómatas celulares</t>
+  </si>
+  <si>
+    <t>Fase 4: Validación del algoritmo en diferentes entornos topológicos</t>
+  </si>
+  <si>
+    <t>12. Implementación de herramienta para aplicar cambios de topología</t>
+  </si>
+  <si>
+    <t>Diseño de reglas probabilísticas</t>
+  </si>
+  <si>
+    <t>Implementación de reglas de comportamiento</t>
+  </si>
+  <si>
+    <t>Simulación del comportamiento de la enfermedad</t>
+  </si>
+  <si>
+    <t>Obtención de datos para el algoritmo en redes neuronales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Análisis del impacto de la condición de frontera </t>
+  </si>
+  <si>
+    <t>Revisión de métodos de clasificación en redes neuronales</t>
+  </si>
+  <si>
+    <t>Definición de métricas para el algoritmo en redes neuronales</t>
+  </si>
+  <si>
+    <t>Implementación de herramienta para aplicar cambios de topología</t>
+  </si>
+  <si>
+    <t>Cambios de topología sobre la simulación en autómatas celulares</t>
+  </si>
+  <si>
+    <t>Redacción del documento final del trabajo de grado</t>
+  </si>
+  <si>
+    <t>Diseño e implementación del algoritmo en redes neuronales sobre datos simulados</t>
+  </si>
+  <si>
+    <t>Validación del comportamiento del algoritmo con datos simulados</t>
+  </si>
+  <si>
+    <t>Validación del algoritmo en redes neuronales con datos obtenidos de los cambios de topología</t>
+  </si>
+  <si>
+    <t>1. Revisión de modelos compartiméntales</t>
+  </si>
+  <si>
+    <t>Fase 2: Análisis sobre la simulación de la enfermedad y comparación con modelos compartiméntales clásicos</t>
+  </si>
+  <si>
+    <t>7. Comparación con modelos compartiméntales clásicos</t>
+  </si>
+  <si>
+    <t>14. Validación del algoritmo en redes neuronales con datos obtenidos de diferentes cambios de topología</t>
+  </si>
+  <si>
+    <t>Revisión de modelos compartiméntales</t>
+  </si>
+  <si>
+    <t>Comparación con modelos compartiméntales clásicos</t>
+  </si>
+  <si>
+    <t>Fase 3: Diseño e implementación del algoritmo en redes neuronales sobre datos simulados</t>
   </si>
 </sst>
 </file>
@@ -174,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,54 +272,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,286 +665,468 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84864F12-16F8-4874-A9CA-C12D1C5A9563}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="16"/>
-    <col min="2" max="2" width="80.140625" customWidth="1"/>
-    <col min="3" max="18" width="3.140625" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" style="16"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="89.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="18" width="3.140625" style="16" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" style="14"/>
+    <col min="20" max="16384" width="11.42578125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="2:18" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
-      <c r="C2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="B3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="18">
         <v>1</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="18">
         <v>2</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="18">
         <v>3</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="18">
         <v>4</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="18">
         <v>5</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="18">
         <v>6</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="18">
         <v>7</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="18">
         <v>8</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="18">
         <v>9</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="18">
         <v>10</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="18">
         <v>11</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="18">
         <v>12</v>
       </c>
-      <c r="O3" s="12">
+      <c r="O3" s="18">
         <v>13</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="18">
         <v>14</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="Q3" s="18">
         <v>15</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="18">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
+      <c r="B4" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
+      <c r="B5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
+      <c r="B6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
+      <c r="B7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
+      <c r="B8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
+      <c r="B9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
+      <c r="B10" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
+      <c r="B11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-    </row>
-    <row r="13" spans="2:18" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:18" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B12" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+    </row>
+    <row r="13" spans="2:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+    </row>
+    <row r="14" spans="2:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:R2"/>
@@ -849,87 +1137,202 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76537682-F71D-4A27-9895-FC61EB096482}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
-    <col min="2" max="2" width="74.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="2"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="5"/>
+    <col min="2" max="2" width="72.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="44.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="5"/>
+    <col min="5" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="13"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="13"/>
+    </row>
+    <row r="27" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="13"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C24:C27"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementación del método de Euler
</commit_message>
<xml_diff>
--- a/Documentos/Elementos.xlsx
+++ b/Documentos/Elementos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tesis\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E8470E-76B4-4CBA-B5E5-E9EC97C82AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB41D77-F421-4467-AB46-B944B388F8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{235F467F-1802-4911-823F-393BAAD41149}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="19440" windowHeight="12165" xr2:uid="{235F467F-1802-4911-823F-393BAAD41149}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Fases Metodológicas</t>
   </si>
@@ -182,13 +182,19 @@
   </si>
   <si>
     <t>Fase 4: Validación del algoritmo frente a cambios de topología</t>
+  </si>
+  <si>
+    <t>SIS, SIR y AC</t>
+  </si>
+  <si>
+    <t>1. Resultados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +210,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +259,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -350,6 +370,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84864F12-16F8-4874-A9CA-C12D1C5A9563}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y23" sqref="Y23"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,10 +1118,12 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="C20" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -1114,8 +1143,10 @@
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="G21" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="21"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -1127,11 +1158,15 @@
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
     </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N25" s="23"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>